<commit_message>
Due to incompatibility between visdcc and the latest dah-plotly-flask modules some functionality was disabled for the time being. We hope to sort this out some time.
 * subplots use the visdcc module to enable hovering data display simultaneously on all subplots - this was disabled
 * Clicking the tab used to update the graphs in the tab - this was used to update the data when the x-slider was changed. This functionality seems to have disappeared in updated modules. We will have to investigate another method to update the graphs in a tab. For the time being the xslider functionality was removed from the graphs.
</commit_message>
<xml_diff>
--- a/dash-config.xlsx
+++ b/dash-config.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23029"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\Technical\Denel\ossim\ossim64bit\green\red\user\tools\python\dash-lineplot\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\Utilities\Python\dash-lineplot\opcode\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E320AD4F-9A41-4FBB-A974-DAEF6D9EECDC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22305" windowHeight="11610" tabRatio="686" firstSheet="2" activeTab="7"/>
+    <workbookView xWindow="13303" yWindow="2194" windowWidth="19337" windowHeight="15609" tabRatio="686" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="header" sheetId="1" r:id="rId1"/>
@@ -488,7 +489,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -949,21 +950,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" style="21" customWidth="1"/>
-    <col min="2" max="2" width="78.140625" style="19" customWidth="1"/>
-    <col min="3" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="14.84375" style="21" customWidth="1"/>
+    <col min="2" max="2" width="78.15234375" style="19" customWidth="1"/>
+    <col min="3" max="16384" width="9.15234375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
@@ -971,7 +972,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A2" s="22" t="s">
         <v>2</v>
       </c>
@@ -979,7 +980,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A3" s="22" t="s">
         <v>87</v>
       </c>
@@ -987,7 +988,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" ht="102" x14ac:dyDescent="0.4">
       <c r="A4" s="22" t="s">
         <v>86</v>
       </c>
@@ -995,7 +996,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A5" s="24" t="s">
         <v>20</v>
       </c>
@@ -1010,27 +1011,27 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:L17"/>
   <sheetViews>
     <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="18.42578125" style="13" customWidth="1"/>
-    <col min="2" max="2" width="66.7109375" style="14" customWidth="1"/>
+    <col min="1" max="1" width="18.3828125" style="13" customWidth="1"/>
+    <col min="2" max="2" width="66.69140625" style="14" customWidth="1"/>
     <col min="3" max="3" width="11" style="14" customWidth="1"/>
-    <col min="4" max="7" width="9.140625" style="2"/>
-    <col min="8" max="8" width="12.42578125" style="2" customWidth="1"/>
-    <col min="9" max="10" width="9.140625" style="2"/>
-    <col min="11" max="11" width="13.5703125" style="2" customWidth="1"/>
-    <col min="12" max="12" width="16.85546875" style="2" customWidth="1"/>
-    <col min="13" max="16384" width="9.140625" style="2"/>
+    <col min="4" max="7" width="9.15234375" style="2"/>
+    <col min="8" max="8" width="12.3828125" style="2" customWidth="1"/>
+    <col min="9" max="10" width="9.15234375" style="2"/>
+    <col min="11" max="11" width="13.53515625" style="2" customWidth="1"/>
+    <col min="12" max="12" width="16.84375" style="2" customWidth="1"/>
+    <col min="13" max="16384" width="9.15234375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
@@ -1068,7 +1069,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A2" s="18" t="s">
         <v>4</v>
       </c>
@@ -1086,7 +1087,7 @@
       <c r="K2" s="3"/>
       <c r="L2" s="3"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A3" s="18" t="s">
         <v>20</v>
       </c>
@@ -1104,7 +1105,7 @@
       <c r="K3" s="3"/>
       <c r="L3" s="3"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A4" s="18" t="s">
         <v>44</v>
       </c>
@@ -1122,7 +1123,7 @@
       <c r="K4" s="3"/>
       <c r="L4" s="3"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A5" s="18" t="s">
         <v>5</v>
       </c>
@@ -1140,7 +1141,7 @@
       <c r="K5" s="3"/>
       <c r="L5" s="3"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A6" s="10" t="s">
         <v>129</v>
       </c>
@@ -1156,7 +1157,7 @@
       <c r="K6" s="3"/>
       <c r="L6" s="3"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A7" s="18" t="s">
         <v>3</v>
       </c>
@@ -1174,7 +1175,7 @@
       <c r="K7" s="3"/>
       <c r="L7" s="3"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A8" s="18" t="s">
         <v>45</v>
       </c>
@@ -1192,7 +1193,7 @@
       <c r="K8" s="3"/>
       <c r="L8" s="3"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A9" s="18" t="s">
         <v>7</v>
       </c>
@@ -1220,7 +1221,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A10" s="18" t="s">
         <v>7</v>
       </c>
@@ -1250,7 +1251,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A11" s="18" t="s">
         <v>7</v>
       </c>
@@ -1278,7 +1279,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A12" s="18" t="s">
         <v>7</v>
       </c>
@@ -1306,7 +1307,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:12" ht="60" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" ht="58.3" x14ac:dyDescent="0.4">
       <c r="A13" s="10" t="s">
         <v>88</v>
       </c>
@@ -1315,7 +1316,7 @@
       </c>
       <c r="C13" s="2"/>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A14" s="10" t="s">
         <v>89</v>
       </c>
@@ -1324,7 +1325,7 @@
       </c>
       <c r="C14" s="2"/>
     </row>
-    <row r="15" spans="1:12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A15" s="10" t="s">
         <v>107</v>
       </c>
@@ -1332,15 +1333,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A16" s="10" t="s">
         <v>109</v>
       </c>
       <c r="B16" s="23" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A17" s="10" t="s">
         <v>139</v>
       </c>
@@ -1350,7 +1351,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="H9" r:id="rId1" display="https://www.w3schools.com/colors/color_tryit.asp?color=BlueViolet"/>
+    <hyperlink ref="H9" r:id="rId1" display="https://www.w3schools.com/colors/color_tryit.asp?color=BlueViolet" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
@@ -1358,21 +1359,21 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:L16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="2" max="2" width="82" customWidth="1"/>
-    <col min="3" max="4" width="14.28515625" customWidth="1"/>
-    <col min="12" max="12" width="14.7109375" customWidth="1"/>
+    <col min="3" max="4" width="14.3046875" customWidth="1"/>
+    <col min="12" max="12" width="14.69140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1410,7 +1411,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A2" s="4" t="s">
         <v>4</v>
       </c>
@@ -1428,7 +1429,7 @@
       <c r="K2" s="3"/>
       <c r="L2" s="3"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A3" s="4" t="s">
         <v>20</v>
       </c>
@@ -1446,7 +1447,7 @@
       <c r="K3" s="3"/>
       <c r="L3" s="3"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A4" s="4" t="s">
         <v>44</v>
       </c>
@@ -1466,7 +1467,7 @@
       <c r="K4" s="3"/>
       <c r="L4" s="3"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A5" s="4" t="s">
         <v>5</v>
       </c>
@@ -1484,7 +1485,7 @@
       <c r="K5" s="3"/>
       <c r="L5" s="3"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A6" s="4" t="s">
         <v>3</v>
       </c>
@@ -1502,7 +1503,7 @@
       <c r="K6" s="3"/>
       <c r="L6" s="3"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A7" s="4" t="s">
         <v>45</v>
       </c>
@@ -1522,7 +1523,7 @@
       <c r="K7" s="3"/>
       <c r="L7" s="3"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A8" s="4" t="s">
         <v>7</v>
       </c>
@@ -1540,7 +1541,7 @@
       <c r="K8" s="5"/>
       <c r="L8" s="5"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A9" s="4" t="s">
         <v>7</v>
       </c>
@@ -1558,7 +1559,7 @@
       <c r="K9" s="5"/>
       <c r="L9" s="5"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A10" s="4" t="s">
         <v>7</v>
       </c>
@@ -1576,7 +1577,7 @@
       <c r="K10" s="5"/>
       <c r="L10" s="5"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A11" s="4" t="s">
         <v>7</v>
       </c>
@@ -1594,7 +1595,7 @@
       <c r="K11" s="5"/>
       <c r="L11" s="5"/>
     </row>
-    <row r="12" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A12" s="10" t="s">
         <v>88</v>
       </c>
@@ -1602,7 +1603,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A13" s="10" t="s">
         <v>89</v>
       </c>
@@ -1610,7 +1611,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A14" s="10" t="s">
         <v>107</v>
       </c>
@@ -1618,7 +1619,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A15" s="10" t="s">
         <v>109</v>
       </c>
@@ -1626,7 +1627,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A16" s="10" t="s">
         <v>139</v>
       </c>
@@ -1640,22 +1641,22 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:L12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7:C8"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="14.140625" customWidth="1"/>
+    <col min="1" max="1" width="14.15234375" customWidth="1"/>
     <col min="2" max="2" width="23" customWidth="1"/>
-    <col min="3" max="4" width="13.85546875" customWidth="1"/>
-    <col min="12" max="12" width="16.28515625" customWidth="1"/>
+    <col min="3" max="4" width="13.84375" customWidth="1"/>
+    <col min="12" max="12" width="16.3046875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1693,7 +1694,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A2" s="4" t="s">
         <v>4</v>
       </c>
@@ -1711,7 +1712,7 @@
       <c r="K2" s="3"/>
       <c r="L2" s="3"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A3" s="4" t="s">
         <v>20</v>
       </c>
@@ -1729,7 +1730,7 @@
       <c r="K3" s="3"/>
       <c r="L3" s="3"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A4" s="4" t="s">
         <v>44</v>
       </c>
@@ -1749,7 +1750,7 @@
       <c r="K4" s="3"/>
       <c r="L4" s="3"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A5" s="4" t="s">
         <v>5</v>
       </c>
@@ -1767,7 +1768,7 @@
       <c r="K5" s="3"/>
       <c r="L5" s="3"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A6" s="10" t="s">
         <v>129</v>
       </c>
@@ -1785,7 +1786,7 @@
       <c r="K6" s="3"/>
       <c r="L6" s="3"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A7" s="4" t="s">
         <v>3</v>
       </c>
@@ -1803,7 +1804,7 @@
       <c r="K7" s="3"/>
       <c r="L7" s="3"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A8" s="4" t="s">
         <v>45</v>
       </c>
@@ -1823,7 +1824,7 @@
       <c r="K8" s="3"/>
       <c r="L8" s="3"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A9" s="4" t="s">
         <v>7</v>
       </c>
@@ -1841,7 +1842,7 @@
       <c r="K9" s="5"/>
       <c r="L9" s="5"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A10" s="10" t="s">
         <v>107</v>
       </c>
@@ -1849,7 +1850,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A11" s="10" t="s">
         <v>109</v>
       </c>
@@ -1857,7 +1858,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A12" s="10" t="s">
         <v>139</v>
       </c>
@@ -1871,21 +1872,21 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:L14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="2" max="2" width="26.85546875" customWidth="1"/>
-    <col min="3" max="4" width="14.28515625" customWidth="1"/>
-    <col min="12" max="12" width="15.85546875" customWidth="1"/>
+    <col min="2" max="2" width="26.84375" customWidth="1"/>
+    <col min="3" max="4" width="14.3046875" customWidth="1"/>
+    <col min="12" max="12" width="15.84375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1923,7 +1924,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A2" s="4" t="s">
         <v>4</v>
       </c>
@@ -1941,7 +1942,7 @@
       <c r="K2" s="3"/>
       <c r="L2" s="3"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A3" s="4" t="s">
         <v>20</v>
       </c>
@@ -1959,7 +1960,7 @@
       <c r="K3" s="3"/>
       <c r="L3" s="3"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A4" s="4" t="s">
         <v>44</v>
       </c>
@@ -1977,7 +1978,7 @@
       <c r="K4" s="3"/>
       <c r="L4" s="3"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A5" s="4" t="s">
         <v>5</v>
       </c>
@@ -1995,7 +1996,7 @@
       <c r="K5" s="3"/>
       <c r="L5" s="3"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A6" s="10" t="s">
         <v>129</v>
       </c>
@@ -2013,7 +2014,7 @@
       <c r="K6" s="3"/>
       <c r="L6" s="3"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A7" s="4" t="s">
         <v>3</v>
       </c>
@@ -2031,7 +2032,7 @@
       <c r="K7" s="3"/>
       <c r="L7" s="3"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A8" s="4" t="s">
         <v>45</v>
       </c>
@@ -2049,7 +2050,7 @@
       <c r="K8" s="3"/>
       <c r="L8" s="3"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A9" s="4" t="s">
         <v>7</v>
       </c>
@@ -2069,7 +2070,7 @@
       <c r="K9" s="5"/>
       <c r="L9" s="5"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A10" s="4" t="s">
         <v>7</v>
       </c>
@@ -2089,7 +2090,7 @@
       <c r="K10" s="5"/>
       <c r="L10" s="5"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A11" s="4" t="s">
         <v>7</v>
       </c>
@@ -2109,7 +2110,7 @@
       <c r="K11" s="5"/>
       <c r="L11" s="5"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A12" s="10" t="s">
         <v>107</v>
       </c>
@@ -2117,7 +2118,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A13" s="10" t="s">
         <v>109</v>
       </c>
@@ -2125,7 +2126,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A14" s="10" t="s">
         <v>139</v>
       </c>
@@ -2139,21 +2140,21 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:L17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="2" max="2" width="26.85546875" customWidth="1"/>
-    <col min="3" max="5" width="14.28515625" customWidth="1"/>
-    <col min="12" max="12" width="15.5703125" customWidth="1"/>
+    <col min="2" max="2" width="26.84375" customWidth="1"/>
+    <col min="3" max="5" width="14.3046875" customWidth="1"/>
+    <col min="12" max="12" width="15.53515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -2191,7 +2192,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A2" s="4" t="s">
         <v>4</v>
       </c>
@@ -2209,7 +2210,7 @@
       <c r="K2" s="3"/>
       <c r="L2" s="3"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A3" s="4" t="s">
         <v>20</v>
       </c>
@@ -2227,7 +2228,7 @@
       <c r="K3" s="3"/>
       <c r="L3" s="3"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A4" s="4" t="s">
         <v>44</v>
       </c>
@@ -2245,7 +2246,7 @@
       <c r="K4" s="3"/>
       <c r="L4" s="3"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A5" s="4" t="s">
         <v>5</v>
       </c>
@@ -2263,7 +2264,7 @@
       <c r="K5" s="3"/>
       <c r="L5" s="3"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A6" s="10" t="s">
         <v>129</v>
       </c>
@@ -2281,7 +2282,7 @@
       <c r="K6" s="3"/>
       <c r="L6" s="3"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A7" s="4" t="s">
         <v>3</v>
       </c>
@@ -2299,7 +2300,7 @@
       <c r="K7" s="3"/>
       <c r="L7" s="3"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A8" s="4" t="s">
         <v>45</v>
       </c>
@@ -2319,7 +2320,7 @@
       <c r="K8" s="3"/>
       <c r="L8" s="3"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A9" s="4" t="s">
         <v>7</v>
       </c>
@@ -2339,7 +2340,7 @@
       <c r="K9" s="5"/>
       <c r="L9" s="5"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A10" s="4" t="s">
         <v>7</v>
       </c>
@@ -2359,7 +2360,7 @@
       <c r="K10" s="5"/>
       <c r="L10" s="5"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A11" s="4" t="s">
         <v>7</v>
       </c>
@@ -2379,7 +2380,7 @@
       <c r="K11" s="5"/>
       <c r="L11" s="5"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A12" s="4" t="s">
         <v>7</v>
       </c>
@@ -2401,7 +2402,7 @@
       <c r="K12" s="5"/>
       <c r="L12" s="5"/>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A13" s="4" t="s">
         <v>7</v>
       </c>
@@ -2421,7 +2422,7 @@
       <c r="K13" s="5"/>
       <c r="L13" s="5"/>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A14" s="4" t="s">
         <v>7</v>
       </c>
@@ -2441,7 +2442,7 @@
       <c r="K14" s="5"/>
       <c r="L14" s="5"/>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A15" s="10" t="s">
         <v>107</v>
       </c>
@@ -2449,7 +2450,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A16" s="10" t="s">
         <v>109</v>
       </c>
@@ -2457,7 +2458,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A17" s="10" t="s">
         <v>139</v>
       </c>
@@ -2471,23 +2472,23 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:L22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="18.7109375" customWidth="1"/>
-    <col min="2" max="2" width="36.140625" customWidth="1"/>
-    <col min="3" max="5" width="14.28515625" customWidth="1"/>
-    <col min="11" max="11" width="14.28515625" customWidth="1"/>
-    <col min="12" max="12" width="15.28515625" customWidth="1"/>
+    <col min="1" max="1" width="18.69140625" customWidth="1"/>
+    <col min="2" max="2" width="36.15234375" customWidth="1"/>
+    <col min="3" max="5" width="14.3046875" customWidth="1"/>
+    <col min="11" max="11" width="14.3046875" customWidth="1"/>
+    <col min="12" max="12" width="15.3046875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -2525,7 +2526,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A2" s="4" t="s">
         <v>4</v>
       </c>
@@ -2543,7 +2544,7 @@
       <c r="K2" s="3"/>
       <c r="L2" s="3"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A3" s="4" t="s">
         <v>20</v>
       </c>
@@ -2561,7 +2562,7 @@
       <c r="K3" s="3"/>
       <c r="L3" s="3"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A4" s="4" t="s">
         <v>44</v>
       </c>
@@ -2579,7 +2580,7 @@
       <c r="K4" s="3"/>
       <c r="L4" s="3"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A5" s="4" t="s">
         <v>5</v>
       </c>
@@ -2597,7 +2598,7 @@
       <c r="K5" s="3"/>
       <c r="L5" s="3"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A6" s="10" t="s">
         <v>129</v>
       </c>
@@ -2615,7 +2616,7 @@
       <c r="K6" s="3"/>
       <c r="L6" s="3"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A7" s="4" t="s">
         <v>3</v>
       </c>
@@ -2633,7 +2634,7 @@
       <c r="K7" s="3"/>
       <c r="L7" s="3"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A8" s="4" t="s">
         <v>45</v>
       </c>
@@ -2651,7 +2652,7 @@
       <c r="K8" s="3"/>
       <c r="L8" s="3"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A9" s="4" t="s">
         <v>7</v>
       </c>
@@ -2675,7 +2676,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A10" s="4" t="s">
         <v>7</v>
       </c>
@@ -2695,7 +2696,7 @@
       <c r="K10" s="5"/>
       <c r="L10" s="5"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A11" s="4" t="s">
         <v>7</v>
       </c>
@@ -2715,7 +2716,7 @@
       <c r="K11" s="5"/>
       <c r="L11" s="5"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A12" s="4" t="s">
         <v>7</v>
       </c>
@@ -2737,7 +2738,7 @@
       <c r="K12" s="5"/>
       <c r="L12" s="5"/>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A13" s="4" t="s">
         <v>7</v>
       </c>
@@ -2757,7 +2758,7 @@
       <c r="K13" s="5"/>
       <c r="L13" s="5"/>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A14" s="4" t="s">
         <v>7</v>
       </c>
@@ -2777,7 +2778,7 @@
       <c r="K14" s="5"/>
       <c r="L14" s="5"/>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A15" s="4" t="s">
         <v>3</v>
       </c>
@@ -2795,7 +2796,7 @@
       <c r="K15" s="3"/>
       <c r="L15" s="3"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A16" s="4" t="s">
         <v>45</v>
       </c>
@@ -2813,7 +2814,7 @@
       <c r="K16" s="3"/>
       <c r="L16" s="3"/>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A17" s="4" t="s">
         <v>7</v>
       </c>
@@ -2837,7 +2838,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A18" s="4" t="s">
         <v>7</v>
       </c>
@@ -2857,7 +2858,7 @@
       <c r="K18" s="5"/>
       <c r="L18" s="5"/>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A19" s="4" t="s">
         <v>7</v>
       </c>
@@ -2877,23 +2878,23 @@
       <c r="K19" s="5"/>
       <c r="L19" s="5"/>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A20" s="10" t="s">
         <v>107</v>
       </c>
       <c r="B20" s="23" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A21" s="10" t="s">
         <v>109</v>
       </c>
       <c r="B21" s="23" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A22" s="10" t="s">
         <v>139</v>
       </c>
@@ -2907,23 +2908,23 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:L22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15:C16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="18.7109375" customWidth="1"/>
-    <col min="2" max="2" width="36.140625" customWidth="1"/>
-    <col min="3" max="5" width="14.28515625" customWidth="1"/>
+    <col min="1" max="1" width="18.69140625" customWidth="1"/>
+    <col min="2" max="2" width="36.15234375" customWidth="1"/>
+    <col min="3" max="5" width="14.3046875" customWidth="1"/>
     <col min="11" max="11" width="14" customWidth="1"/>
-    <col min="12" max="12" width="15.28515625" customWidth="1"/>
+    <col min="12" max="12" width="15.3046875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -2961,7 +2962,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A2" s="4" t="s">
         <v>4</v>
       </c>
@@ -2979,7 +2980,7 @@
       <c r="K2" s="3"/>
       <c r="L2" s="3"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A3" s="4" t="s">
         <v>20</v>
       </c>
@@ -2997,7 +2998,7 @@
       <c r="K3" s="3"/>
       <c r="L3" s="3"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A4" s="4" t="s">
         <v>44</v>
       </c>
@@ -3017,7 +3018,7 @@
       <c r="K4" s="3"/>
       <c r="L4" s="3"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A5" s="4" t="s">
         <v>5</v>
       </c>
@@ -3035,7 +3036,7 @@
       <c r="K5" s="3"/>
       <c r="L5" s="3"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A6" s="10" t="s">
         <v>129</v>
       </c>
@@ -3053,7 +3054,7 @@
       <c r="K6" s="3"/>
       <c r="L6" s="3"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A7" s="4" t="s">
         <v>3</v>
       </c>
@@ -3071,7 +3072,7 @@
       <c r="K7" s="3"/>
       <c r="L7" s="3"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A8" s="4" t="s">
         <v>45</v>
       </c>
@@ -3091,7 +3092,7 @@
       <c r="K8" s="3"/>
       <c r="L8" s="3"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A9" s="4" t="s">
         <v>7</v>
       </c>
@@ -3115,7 +3116,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A10" s="4" t="s">
         <v>7</v>
       </c>
@@ -3135,7 +3136,7 @@
       <c r="K10" s="5"/>
       <c r="L10" s="5"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A11" s="4" t="s">
         <v>7</v>
       </c>
@@ -3155,7 +3156,7 @@
       <c r="K11" s="5"/>
       <c r="L11" s="5"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A12" s="4" t="s">
         <v>7</v>
       </c>
@@ -3177,7 +3178,7 @@
       <c r="K12" s="5"/>
       <c r="L12" s="5"/>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A13" s="4" t="s">
         <v>7</v>
       </c>
@@ -3197,7 +3198,7 @@
       <c r="K13" s="5"/>
       <c r="L13" s="5"/>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A14" s="4" t="s">
         <v>7</v>
       </c>
@@ -3217,7 +3218,7 @@
       <c r="K14" s="5"/>
       <c r="L14" s="5"/>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A15" s="4" t="s">
         <v>3</v>
       </c>
@@ -3235,7 +3236,7 @@
       <c r="K15" s="3"/>
       <c r="L15" s="3"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A16" s="4" t="s">
         <v>45</v>
       </c>
@@ -3255,7 +3256,7 @@
       <c r="K16" s="3"/>
       <c r="L16" s="3"/>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A17" s="4" t="s">
         <v>7</v>
       </c>
@@ -3279,7 +3280,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A18" s="4" t="s">
         <v>7</v>
       </c>
@@ -3299,7 +3300,7 @@
       <c r="K18" s="5"/>
       <c r="L18" s="5"/>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A19" s="4" t="s">
         <v>7</v>
       </c>
@@ -3319,7 +3320,7 @@
       <c r="K19" s="5"/>
       <c r="L19" s="5"/>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A20" s="10" t="s">
         <v>107</v>
       </c>
@@ -3327,20 +3328,20 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A21" s="10" t="s">
         <v>109</v>
       </c>
       <c r="B21" s="23" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A22" s="10" t="s">
         <v>139</v>
       </c>
       <c r="B22" s="23" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -3349,39 +3350,39 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:AMK55"/>
   <sheetViews>
     <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="19.7109375" style="13" customWidth="1"/>
-    <col min="2" max="2" width="70.28515625" style="8" customWidth="1"/>
-    <col min="3" max="16384" width="9.140625" style="2"/>
+    <col min="1" max="1" width="19.69140625" style="13" customWidth="1"/>
+    <col min="2" max="2" width="70.3046875" style="8" customWidth="1"/>
+    <col min="3" max="16384" width="9.15234375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1025" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1025" x14ac:dyDescent="0.4">
       <c r="A1" s="7"/>
       <c r="B1" s="8" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="2" spans="1:1025" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1025" x14ac:dyDescent="0.4">
       <c r="A2" s="9"/>
       <c r="B2" s="8" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="3" spans="1:1025" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1025" x14ac:dyDescent="0.4">
       <c r="A3" s="10"/>
       <c r="B3" s="8" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="5" spans="1:1025" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1025" x14ac:dyDescent="0.4">
       <c r="A5" s="7" t="s">
         <v>4</v>
       </c>
@@ -3389,7 +3390,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="6" spans="1:1025" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1025" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A6" s="7" t="s">
         <v>20</v>
       </c>
@@ -3397,7 +3398,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="7" spans="1:1025" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1025" x14ac:dyDescent="0.4">
       <c r="A7" s="7" t="s">
         <v>44</v>
       </c>
@@ -3405,7 +3406,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="8" spans="1:1025" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:1025" x14ac:dyDescent="0.4">
       <c r="A8" s="7" t="s">
         <v>5</v>
       </c>
@@ -3413,13 +3414,13 @@
         <v>78</v>
       </c>
     </row>
-    <row r="9" spans="1:1025" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:1025" x14ac:dyDescent="0.4">
       <c r="A9" s="34" t="s">
         <v>123</v>
       </c>
       <c r="B9" s="34"/>
     </row>
-    <row r="10" spans="1:1025" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:1025" x14ac:dyDescent="0.4">
       <c r="A10" s="10" t="s">
         <v>129</v>
       </c>
@@ -3427,7 +3428,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="11" spans="1:1025" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:1025" x14ac:dyDescent="0.4">
       <c r="A11" s="7" t="s">
         <v>3</v>
       </c>
@@ -3435,7 +3436,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="12" spans="1:1025" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:1025" x14ac:dyDescent="0.4">
       <c r="A12" s="7" t="s">
         <v>45</v>
       </c>
@@ -3443,7 +3444,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="13" spans="1:1025" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:1025" x14ac:dyDescent="0.4">
       <c r="A13" s="7" t="s">
         <v>7</v>
       </c>
@@ -3451,7 +3452,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="15" spans="1:1025" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:1025" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A15" s="10" t="s">
         <v>131</v>
       </c>
@@ -4482,7 +4483,7 @@
       <c r="AMJ15" s="30"/>
       <c r="AMK15" s="30"/>
     </row>
-    <row r="16" spans="1:1025" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:1025" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A16" s="10"/>
       <c r="B16" s="29" t="s">
         <v>133</v>
@@ -5511,7 +5512,7 @@
       <c r="AMJ16" s="30"/>
       <c r="AMK16" s="30"/>
     </row>
-    <row r="17" spans="1:1025" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1025" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A17" s="10"/>
       <c r="B17" s="29" t="s">
         <v>134</v>
@@ -6540,7 +6541,7 @@
       <c r="AMJ17" s="30"/>
       <c r="AMK17" s="30"/>
     </row>
-    <row r="18" spans="1:1025" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1025" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A18" s="10" t="s">
         <v>137</v>
       </c>
@@ -7571,7 +7572,7 @@
       <c r="AMJ18" s="30"/>
       <c r="AMK18" s="30"/>
     </row>
-    <row r="19" spans="1:1025" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1025" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A19" s="10"/>
       <c r="B19" s="29" t="s">
         <v>135</v>
@@ -8600,7 +8601,7 @@
       <c r="AMJ19" s="30"/>
       <c r="AMK19" s="30"/>
     </row>
-    <row r="20" spans="1:1025" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1025" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A20" s="28" t="s">
         <v>124</v>
       </c>
@@ -9631,7 +9632,7 @@
       <c r="AMJ20" s="30"/>
       <c r="AMK20" s="30"/>
     </row>
-    <row r="21" spans="1:1025" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1025" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A21" s="28"/>
       <c r="B21" s="29" t="s">
         <v>142</v>
@@ -10660,7 +10661,7 @@
       <c r="AMJ21" s="30"/>
       <c r="AMK21" s="30"/>
     </row>
-    <row r="22" spans="1:1025" ht="30" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:1025" x14ac:dyDescent="0.4">
       <c r="A22" s="10" t="s">
         <v>52</v>
       </c>
@@ -10668,16 +10669,16 @@
         <v>100</v>
       </c>
     </row>
-    <row r="23" spans="1:1025" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:1025" x14ac:dyDescent="0.4">
       <c r="A23" s="10"/>
       <c r="B23" s="8" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="24" spans="1:1025" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:1025" x14ac:dyDescent="0.4">
       <c r="A24" s="10"/>
     </row>
-    <row r="25" spans="1:1025" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:1025" x14ac:dyDescent="0.4">
       <c r="A25" s="10" t="s">
         <v>53</v>
       </c>
@@ -10685,13 +10686,13 @@
         <v>54</v>
       </c>
     </row>
-    <row r="26" spans="1:1025" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:1025" x14ac:dyDescent="0.4">
       <c r="A26" s="10"/>
       <c r="B26" s="8" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="27" spans="1:1025" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:1025" x14ac:dyDescent="0.4">
       <c r="A27" s="10" t="s">
         <v>102</v>
       </c>
@@ -10699,7 +10700,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="28" spans="1:1025" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:1025" x14ac:dyDescent="0.4">
       <c r="A28" s="10" t="s">
         <v>41</v>
       </c>
@@ -10707,10 +10708,10 @@
         <v>103</v>
       </c>
     </row>
-    <row r="29" spans="1:1025" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:1025" x14ac:dyDescent="0.4">
       <c r="A29" s="10"/>
     </row>
-    <row r="30" spans="1:1025" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:1025" x14ac:dyDescent="0.4">
       <c r="A30" s="10" t="s">
         <v>99</v>
       </c>
@@ -10718,10 +10719,10 @@
         <v>104</v>
       </c>
     </row>
-    <row r="31" spans="1:1025" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:1025" x14ac:dyDescent="0.4">
       <c r="A31" s="10"/>
     </row>
-    <row r="32" spans="1:1025" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:1025" x14ac:dyDescent="0.4">
       <c r="A32" s="10" t="s">
         <v>70</v>
       </c>
@@ -10729,47 +10730,47 @@
         <v>85</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A33" s="10"/>
       <c r="B33" s="8" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A34" s="10"/>
       <c r="B34" s="8" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A35" s="10"/>
       <c r="B35" s="12" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A36" s="10"/>
       <c r="B36" s="12" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A37" s="10"/>
       <c r="B37" s="12" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A38" s="10"/>
       <c r="B38" s="12" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A39" s="10"/>
       <c r="B39" s="12"/>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A40" s="10" t="s">
         <v>68</v>
       </c>
@@ -10777,17 +10778,17 @@
         <v>105</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A41" s="10"/>
       <c r="B41" s="12" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A42" s="10"/>
       <c r="B42" s="12"/>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A43" s="10" t="s">
         <v>67</v>
       </c>
@@ -10795,16 +10796,16 @@
         <v>73</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A44" s="10"/>
       <c r="B44" s="8" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A45" s="10"/>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A46" s="10" t="s">
         <v>88</v>
       </c>
@@ -10812,10 +10813,10 @@
         <v>92</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A47" s="10"/>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A48" s="10" t="s">
         <v>89</v>
       </c>
@@ -10823,10 +10824,10 @@
         <v>93</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A49" s="10"/>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A50" s="10" t="s">
         <v>107</v>
       </c>
@@ -10834,10 +10835,10 @@
         <v>108</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A51" s="10"/>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A52" s="10" t="s">
         <v>109</v>
       </c>
@@ -10845,7 +10846,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="53" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A53" s="10" t="s">
         <v>139</v>
       </c>
@@ -10853,10 +10854,10 @@
         <v>140</v>
       </c>
     </row>
-    <row r="54" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A54" s="33"/>
     </row>
-    <row r="55" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:2" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A55" s="13" t="s">
         <v>83</v>
       </c>
@@ -10869,9 +10870,9 @@
     <mergeCell ref="A9:B9"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="B35" r:id="rId1"/>
-    <hyperlink ref="B36" r:id="rId2"/>
-    <hyperlink ref="B37" r:id="rId3"/>
+    <hyperlink ref="B35" r:id="rId1" xr:uid="{00000000-0004-0000-0800-000000000000}"/>
+    <hyperlink ref="B36" r:id="rId2" xr:uid="{00000000-0004-0000-0800-000001000000}"/>
+    <hyperlink ref="B37" r:id="rId3" xr:uid="{00000000-0004-0000-0800-000002000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>

</xml_diff>